<commit_message>
Added 'Region' to location table, create temporary CSV of data, and completed half of seed script
</commit_message>
<xml_diff>
--- a/CanadianDisasterDatabase.xlsx
+++ b/CanadianDisasterDatabase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathangratton/OneDrive/University of Ottawa/Winter 2018/CSI 4142 - Introduction to Data Science/DisasterMart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0898E70-0E17-F941-B373-92475CF0B796}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB324D2-691C-3747-AAB3-7BFBAAB6C691}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6119,7 +6119,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="27" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="yyyy/mm/dd\ h:mm"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -6130,6 +6137,37 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{903E3474-E6A6-0747-9139-41978CDD5C84}" name="Table1" displayName="Table1" ref="A1:V1090" totalsRowShown="0">
+  <autoFilter ref="A1:V1090" xr:uid="{ACBC40BE-572C-944E-8032-8B1FC9FAAF3C}"/>
+  <tableColumns count="22">
+    <tableColumn id="1" xr3:uid="{8DC1BA4C-E85A-8047-992F-F59A81FE6BC4}" name="EVENT CATEGORY"/>
+    <tableColumn id="2" xr3:uid="{B38BE625-C8E3-6540-A43C-B3A1B29814F0}" name="EVENT GROUP"/>
+    <tableColumn id="3" xr3:uid="{3FD24EE0-1EAE-094E-AC30-AFDCCC076A53}" name="EVENT SUBGROUP"/>
+    <tableColumn id="4" xr3:uid="{4F3B1326-AC23-9E4E-9029-638E3A17FBC7}" name="EVENT TYPE"/>
+    <tableColumn id="5" xr3:uid="{7C224BD1-7271-7949-8D20-1082A458A50B}" name="PLACE"/>
+    <tableColumn id="6" xr3:uid="{4AE68672-A9C6-5D4D-BECC-27593C6A048D}" name="EVENT START DATE" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{4474F36F-5463-8844-8D80-7B538A371EF1}" name="COMMENTS"/>
+    <tableColumn id="8" xr3:uid="{12B8A3F1-ED25-BB4A-8E19-6A72C954987F}" name="FATALITIES"/>
+    <tableColumn id="9" xr3:uid="{478A6D1B-B496-6440-8CE1-377532431ED7}" name="INJURED / INFECTED"/>
+    <tableColumn id="10" xr3:uid="{D3B02F14-73EC-1E44-B0C2-B91FA24CF10F}" name="EVACUATED"/>
+    <tableColumn id="11" xr3:uid="{2565B81E-F6D5-C140-9068-C6115DA1EAB3}" name="ESTIMATED TOTAL COST"/>
+    <tableColumn id="12" xr3:uid="{3C11A051-B835-084C-997E-E62B747F9FCB}" name="NORMALIZED TOTAL COST"/>
+    <tableColumn id="13" xr3:uid="{2E2C488A-8553-7148-B506-8860C1A125F3}" name="EVENT END DATE" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{3B8D6E9C-8E4B-9348-82B9-A998AF4F3EA8}" name="FEDERAL DFAA PAYMENTS"/>
+    <tableColumn id="15" xr3:uid="{F555CD6F-6D7B-6C45-86AE-C9C7D8A419C6}" name="PROVINCIAL DFAA PAYMENTS"/>
+    <tableColumn id="16" xr3:uid="{2CCCB3A4-6BCC-334F-8A41-5A6A83CB571A}" name="PROVINCIAL DEPARTMENT PAYMENTS"/>
+    <tableColumn id="17" xr3:uid="{3D66AC4B-B705-CA43-9B29-87F759863E71}" name="MUNICIPAL COSTS"/>
+    <tableColumn id="18" xr3:uid="{F861D68B-0CEE-4C42-9788-B52F8186052F}" name="OGD COSTS"/>
+    <tableColumn id="19" xr3:uid="{6E9CB78F-6E02-7C4D-861D-3EA5B1A3447F}" name="INSURANCE PAYMENTS"/>
+    <tableColumn id="20" xr3:uid="{A4A9529E-5940-C74B-BB0A-421EF50205B1}" name="NGO PAYMENTS"/>
+    <tableColumn id="21" xr3:uid="{BBB7661A-5230-CA46-884F-8E55BF357947}" name="UTILITY - PEOPLE AFFECTED"/>
+    <tableColumn id="22" xr3:uid="{47935774-6F1C-8A45-B752-68DC923E9D5D}" name="MAGNITUDE"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6397,34 +6435,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1090"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1064" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="A808" zoomScale="173" workbookViewId="0">
+      <selection activeCell="E805" sqref="E805"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="143.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="21.5" customWidth="1"/>
+    <col min="12" max="12" width="23.1640625" customWidth="1"/>
+    <col min="13" max="13" width="16.1640625" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" customWidth="1"/>
+    <col min="15" max="15" width="26.5" customWidth="1"/>
+    <col min="16" max="16" width="32.6640625" customWidth="1"/>
+    <col min="17" max="17" width="17.5" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
+    <col min="19" max="19" width="21.1640625" customWidth="1"/>
+    <col min="20" max="20" width="15.83203125" customWidth="1"/>
+    <col min="21" max="21" width="23.83203125" customWidth="1"/>
+    <col min="22" max="22" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
@@ -56414,5 +56452,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>